<commit_message>
fixed the convection coeff calculator
</commit_message>
<xml_diff>
--- a/ThermalStackFEA Parameters and Material Properties.xlsx
+++ b/ThermalStackFEA Parameters and Material Properties.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C98F1EC2-1425-4D45-BC50-27A84C02D915}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92318A4D-7300-486B-A7B7-872AA62B7CF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Material</t>
   </si>
@@ -124,14 +134,34 @@
   </si>
   <si>
     <t>real values for water are not used in this algorithm, see below</t>
+  </si>
+  <si>
+    <t>Solder</t>
+  </si>
+  <si>
+    <t>mesh size</t>
+  </si>
+  <si>
+    <t>elements</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>Rth</t>
+  </si>
+  <si>
+    <t>ground tru.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -359,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -401,9 +431,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -443,6 +470,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,6 +538,1007 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Element Count</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Case Resistance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:forward val="900000"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>33824</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>249984</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>480200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1942528</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.19600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6401-4AFF-B077-550E061DA59C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="752706216"/>
+        <c:axId val="752708184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="752706216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="752708184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="752708184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="752706216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45637B9E-C693-4262-9DAA-66B0C3CE74A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="C4">
+            <v>33824</v>
+          </cell>
+          <cell r="E4">
+            <v>0.19600000000000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>249984</v>
+          </cell>
+          <cell r="E5">
+            <v>0.16</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>480200</v>
+          </cell>
+          <cell r="E6">
+            <v>0.152</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>1942528</v>
+          </cell>
+          <cell r="E7">
+            <v>0.13800000000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,75 +1804,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L50"/>
+  <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="1.36328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="3.453125" style="3" customWidth="1"/>
-    <col min="4" max="9" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.81640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4.08984375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="36.6328125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="3.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="1.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="3.44140625" style="3" customWidth="1"/>
+    <col min="4" max="9" width="16.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="4" customWidth="1"/>
+    <col min="11" max="12" width="13.88671875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D3" s="13"/>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="7" spans="2:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="D7" s="41" t="s">
+      <c r="J4" s="14"/>
+    </row>
+    <row r="7" spans="2:12" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="10" spans="2:12" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="22"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="44"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="10" spans="2:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
       <c r="D10" s="2" t="s">
         <v>0</v>
       </c>
@@ -864,13 +1897,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="16"/>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="15"/>
       <c r="F11" s="13"/>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="15"/>
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
@@ -891,7 +1924,7 @@
         <f>H12/1000</f>
         <v>2.33E-3</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="14">
         <f>G12*I12</f>
         <v>1.6426499999999998E-3</v>
       </c>
@@ -899,441 +1932,565 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="15"/>
       <c r="D13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="3">
+        <v>59</v>
+      </c>
+      <c r="F13" s="13">
+        <f>E13/1000</f>
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="I13" s="3">
+        <f>H13/1000</f>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="J13" s="14">
+        <f>G13*I13</f>
+        <v>1.554E-3</v>
+      </c>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="15"/>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="3">
         <v>401</v>
       </c>
-      <c r="F13" s="13">
-        <f t="shared" ref="F13:F16" si="0">E13/1000</f>
+      <c r="F14" s="13">
+        <f t="shared" ref="F14:F17" si="0">E14/1000</f>
         <v>0.40100000000000002</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G14" s="3">
         <v>0.38500000000000001</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H14" s="3">
         <v>8.9600000000000009</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" ref="I13:I16" si="1">H13/1000</f>
+      <c r="I14" s="3">
+        <f t="shared" ref="I14:I17" si="1">H14/1000</f>
         <v>8.9600000000000009E-3</v>
       </c>
-      <c r="J13" s="15">
-        <f t="shared" ref="J13:J16" si="2">G13*I13</f>
+      <c r="J14" s="14">
+        <f t="shared" ref="J14:J17" si="2">G14*I14</f>
         <v>3.4496000000000006E-3</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L14" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="D14" s="3" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="15"/>
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E15" s="3">
         <v>205</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F15" s="13">
         <f t="shared" si="0"/>
         <v>0.20499999999999999</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G15" s="3">
         <v>0.89700000000000002</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>2.702</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I15" s="3">
         <f t="shared" si="1"/>
         <v>2.702E-3</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J15" s="14">
         <f t="shared" si="2"/>
         <v>2.4236940000000001E-3</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="16"/>
-      <c r="D15" s="3" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="15"/>
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="3">
-        <v>10</v>
-      </c>
-      <c r="F15" s="13">
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="13">
         <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="G15" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G16" s="3">
         <v>0.88</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <v>3.95</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I16" s="3">
         <f t="shared" si="1"/>
         <v>3.9500000000000004E-3</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J16" s="14">
         <f t="shared" si="2"/>
         <v>3.4760000000000004E-3</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L16" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="16"/>
-      <c r="D16" s="3" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="15"/>
+      <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E17" s="3">
         <v>0.60599999999999998</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F17" s="3">
         <f t="shared" si="0"/>
         <v>6.0599999999999998E-4</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G17" s="3">
         <v>4.1859999999999999</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <v>0.997</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I17" s="3">
         <f t="shared" si="1"/>
         <v>9.9700000000000006E-4</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J17" s="4">
         <f t="shared" si="2"/>
         <v>4.1734420000000003E-3</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L17" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="D21" s="41" t="s">
+    <row r="22" spans="2:12" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="D22" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
-    </row>
-    <row r="22" spans="2:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="D22" s="23"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
-    </row>
-    <row r="24" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="16"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="29" t="s">
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="44"/>
+    </row>
+    <row r="23" spans="2:12" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+    </row>
+    <row r="25" spans="2:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B25" s="16"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="34"/>
-    </row>
-    <row r="26" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="16"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="34"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="16"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="34"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="16"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="34"/>
-    </row>
-    <row r="29" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="11"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="15"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="2:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="15"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="35"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="15"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="35"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="15"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
+    </row>
+    <row r="30" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="11"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="35"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="11"/>
-      <c r="C31" s="21"/>
-      <c r="E31" s="9" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="11"/>
+      <c r="C32" s="20"/>
+      <c r="E32" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="9"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="11"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12">
-        <v>0.5</v>
-      </c>
+      <c r="H32" s="9"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11"/>
-      <c r="C33" s="21"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="11"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="11"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="3" t="s">
+      <c r="G34" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="I34" s="29"/>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="11"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E35" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12">
-        <f>G33/(2 * G32)</f>
-        <v>0.01</v>
-      </c>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F35" s="12"/>
+      <c r="G35" s="12">
+        <f>(G33/2)*G34</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H36" s="29"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="17"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="19"/>
+    <row r="38" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="2:12" s="7" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="11"/>
-      <c r="D39" s="29" t="s">
+    <row r="39" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="16"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="2:12" s="7" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="11"/>
+      <c r="D40" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="11"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="34"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="32"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="11"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="34"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="35"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="11"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="34"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="35"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="11"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="34"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="35"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="34"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="35"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="11"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="35"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="11"/>
-      <c r="E46" s="9" t="s">
+      <c r="D46" s="36"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="11"/>
+      <c r="E47" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="9"/>
-      <c r="L46" s="10"/>
-    </row>
-    <row r="47" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="11"/>
-      <c r="D47" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H47" s="9"/>
+      <c r="L47" s="10"/>
+    </row>
+    <row r="48" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="11"/>
       <c r="D48" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12">
-        <v>50</v>
-      </c>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="11"/>
       <c r="D49" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12">
+        <v>1</v>
+      </c>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="11"/>
+      <c r="D50" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G49" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B50" s="16"/>
-      <c r="D50" s="3" t="s">
+      <c r="G50" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="J50" s="8"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="15"/>
+      <c r="D51" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="14">
-        <f>G49*G48*G47</f>
-        <v>5.0000000000000001E-4</v>
+      <c r="F51" s="13"/>
+      <c r="G51" s="28">
+        <f>G50*G49*G48</f>
+        <v>2.0000000000000002E-7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D39:I45"/>
+    <mergeCell ref="D40:I46"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D24:I30"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="D25:I31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AA9CDB-31B8-4EAC-BB49-A502933EBBFB}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <v>33824</v>
+      </c>
+      <c r="D4">
+        <v>96696</v>
+      </c>
+      <c r="E4">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0.125</v>
+      </c>
+      <c r="C5">
+        <v>249984</v>
+      </c>
+      <c r="D5">
+        <v>731312</v>
+      </c>
+      <c r="E5">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <v>480200</v>
+      </c>
+      <c r="D6">
+        <v>1411620</v>
+      </c>
+      <c r="E6">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C7">
+        <v>1942528</v>
+      </c>
+      <c r="D7">
+        <v>5753504</v>
+      </c>
+      <c r="E7">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>